<commit_message>
updating Luk and Spivak 2020 hook
</commit_message>
<xml_diff>
--- a/data/primary_studies/Luk_2020/intermediate/Luk_et_al_2020_material_and_methods.xlsx
+++ b/data/primary_studies/Luk_2020/intermediate/Luk_et_al_2020_material_and_methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Luk_2020/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE5DF05-7088-3647-8A68-6CE7176B9E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC6C02-05C2-9445-865D-2A21ACE63841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="material_and_methods" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>coring_method</t>
   </si>
@@ -274,12 +274,6 @@
     <t>sediment_sieved_flag</t>
   </si>
   <si>
-    <t>Luk_et_al_2019</t>
-  </si>
-  <si>
-    <t>No obvious compaction</t>
-  </si>
-  <si>
     <t>gamma</t>
   </si>
   <si>
@@ -290,6 +284,18 @@
   </si>
   <si>
     <t>acid fumigation</t>
+  </si>
+  <si>
+    <t>no obvious compaction</t>
+  </si>
+  <si>
+    <t>freeze dried</t>
+  </si>
+  <si>
+    <t>Luk_et_al_2020_a</t>
+  </si>
+  <si>
+    <t>Luk_et_al_2020_b</t>
   </si>
 </sst>
 </file>
@@ -1143,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1416,22 +1422,22 @@
     </row>
     <row r="4" spans="1:31" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E4" s="4">
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G4" s="4">
         <v>60</v>
@@ -1454,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="T4" s="4" t="s">
         <v>81</v>
@@ -1463,12 +1469,8 @@
         <v>80</v>
       </c>
       <c r="V4" s="4"/>
-      <c r="W4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
@@ -1477,6 +1479,53 @@
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
     </row>
+    <row r="5" spans="1:31" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4">
+        <v>168</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding a method_id to mixed method studies and updating the synthesis
</commit_message>
<xml_diff>
--- a/data/primary_studies/Luk_2020/intermediate/Luk_et_al_2020_material_and_methods.xlsx
+++ b/data/primary_studies/Luk_2020/intermediate/Luk_et_al_2020_material_and_methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/Luk_2020/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC6C02-05C2-9445-865D-2A21ACE63841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A2CE3B-1C80-F240-AEFD-966C88D9DAB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="94">
   <si>
     <t>coring_method</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>Luk_et_al_2020_b</t>
+  </si>
+  <si>
+    <t>method_id</t>
+  </si>
+  <si>
+    <t>Luk_et_al_2020</t>
   </si>
 </sst>
 </file>
@@ -1149,326 +1155,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="31" width="34.5" style="2" customWidth="1"/>
+    <col min="2" max="32" width="34.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:32" ht="64" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="D3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>69</v>
       </c>
       <c r="Y3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:32" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>60</v>
       </c>
-      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="4"/>
+      <c r="L4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="R4" s="4" t="b">
+      <c r="S4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
@@ -1478,30 +1489,33 @@
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
     </row>
-    <row r="5" spans="1:31" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:32" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4">
+      <c r="H5" s="4"/>
+      <c r="I5" s="4">
         <v>168</v>
       </c>
-      <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1512,19 +1526,20 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
-      <c r="W5" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="W5" s="4"/>
       <c r="X5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="4"/>
+      <c r="Y5" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>